<commit_message>
deactivated that every spiders writes to excel
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_types.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_types.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9957</v>
+        <v>9958</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1267,11 +1267,11 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1667,11 +1667,11 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1595</v>
+        <v>1597</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1807,11 +1807,11 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1927,11 +1927,11 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2025-05-27</t>
+          <t>2025-05-28</t>
         </is>
       </c>
     </row>

</xml_diff>